<commit_message>
draft of report mostly done, need to cut some stuff out though
</commit_message>
<xml_diff>
--- a/data/motorDistanceChart.xlsx
+++ b/data/motorDistanceChart.xlsx
@@ -5,28 +5,33 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="motorDistance" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>commandedMotorClicks</t>
+    <t xml:space="preserve">commandedMotorClicks</t>
   </si>
   <si>
-    <t>actualMotorClicksL</t>
+    <t xml:space="preserve">actualMotorClicksL</t>
   </si>
   <si>
-    <t>actualMotorClicksR</t>
+    <t xml:space="preserve">actualMotorClicksR</t>
   </si>
   <si>
-    <t>mmTraveled</t>
+    <t xml:space="preserve">mmTraveled</t>
   </si>
 </sst>
 </file>
@@ -34,13 +39,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -58,11 +64,12 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -171,7 +178,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFEE4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -190,29 +197,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Distance traveled at 25% power</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -232,7 +219,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="ee4000"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
@@ -247,6 +234,14 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
@@ -354,11 +349,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="66175455"/>
-        <c:axId val="96768285"/>
+        <c:axId val="38900798"/>
+        <c:axId val="56888744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66175455"/>
+        <c:axId val="38900798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,23 +362,42 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>commandedClicks</a:t>
+                  <a:t>clicksCommanded</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -394,11 +408,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96768285"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56888744"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96768285"/>
+        <c:axId val="56888744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,14 +449,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>mmTraveled</a:t>
@@ -431,8 +482,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -443,8 +495,27 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66175455"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38900798"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -456,6 +527,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -472,16 +544,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>100440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>327960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -489,8 +561,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4743360" y="36000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7339320" y="611640"/>
+        <a:ext cx="4342320" cy="2283480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -511,16 +583,16 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>